<commit_message>
Soil v2.02 and manure 1.0.1 updates
-Clarified TKN vs TN in soil and manure list methods
-Fixed duplicate P and S methods in manure list
-corresponding updates to supersession tables
-added row change data and change comment columns to soil list
</commit_message>
<xml_diff>
--- a/Method Lists/Modus2 Manure Code Supersession.xlsx
+++ b/Method Lists/Modus2 Manure Code Supersession.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aggateway-my.sharepoint.com/personal/ben_craker_aggateway_org/Documents/Working Groups/WG04 Ag Lab Data/The File/Manure/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3acd474740f4845a/Documents/GitHub/Modus/Method Lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3504F47-FF5E-4F6A-92E4-6C905BB1E473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{A3504F47-FF5E-4F6A-92E4-6C905BB1E473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05C61F5A-42A2-47D7-BB5F-4B267FCA51C3}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{774C6DCF-8886-43F7-90F7-36CDF949DA3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="176">
   <si>
     <t>M-5DAYGERM</t>
   </si>
@@ -516,6 +516,54 @@
   </si>
   <si>
     <t>V2 Manure Code (Supersedes to)</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_P_004</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_P_005</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_P_006</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_P_007</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_P_009</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_P_011</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_P_013</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_S_005</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_TKN_002</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_TKN_003</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_TKN_005</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_TKN_006</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_TKN_007</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_TKN_008</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_TN_001</t>
+  </si>
+  <si>
+    <t>L_MODV2_MANURE_TN_002</t>
   </si>
 </sst>
 </file>
@@ -902,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B385C0-D2F5-4B9D-9E57-23648A312D1D}">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,637 +972,744 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>160</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>138</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>153</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>91</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>112</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>136</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>137</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>138</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>156</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>157</v>
       </c>
     </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B93">
+    <sortCondition ref="A64:A93"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>